<commit_message>
Mejorado parseador + añadida encriptación de passwords
</commit_message>
<xml_diff>
--- a/src/test/resources/test1.xlsx
+++ b/src/test/resources/test1.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\git\Loader_e2a\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13035" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19845" windowHeight="5025"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,52 +20,115 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+  <si>
+    <t>Contrasena</t>
+  </si>
+  <si>
+    <t>Nombre_usuario</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>KindCode</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>Correo electrónico</t>
-  </si>
-  <si>
-    <t>Identificador</t>
-  </si>
-  <si>
-    <t>Tipo</t>
+    <t>Apellidos</t>
+  </si>
+  <si>
+    <t>Correo electronico</t>
+  </si>
+  <si>
+    <t>sensor1@sensor.com</t>
+  </si>
+  <si>
+    <t>Soria</t>
+  </si>
+  <si>
+    <t>Pepa</t>
+  </si>
+  <si>
+    <t>219237kyz</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Sensor1</t>
+  </si>
+  <si>
+    <t>Persona1</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>5901927Z</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Rato</t>
+  </si>
+  <si>
+    <t>estafa@hotmail.com</t>
+  </si>
+  <si>
+    <t>Entidad1</t>
   </si>
   <si>
     <t>Entity</t>
   </si>
   <si>
-    <t>sensor2@sensor.com</t>
-  </si>
-  <si>
-    <t>Contrasena</t>
-  </si>
-  <si>
-    <t>KindCode</t>
-  </si>
-  <si>
-    <t>Apellidos</t>
-  </si>
-  <si>
-    <t>Soria</t>
-  </si>
-  <si>
-    <t>skjdfkshgd</t>
-  </si>
-  <si>
-    <t>21487463Y12335jke3</t>
-  </si>
-  <si>
-    <t>asdsabhnhnne3</t>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>Entidad</t>
+  </si>
+  <si>
+    <t>Amarillo</t>
+  </si>
+  <si>
+    <t>entity@hotmail.com</t>
+  </si>
+  <si>
+    <t>Entidad2</t>
+  </si>
+  <si>
+    <t>WWE</t>
+  </si>
+  <si>
+    <t>Rojo</t>
+  </si>
+  <si>
+    <t>entity2@hotmail.com</t>
+  </si>
+  <si>
+    <t>Entidad3</t>
+  </si>
+  <si>
+    <t>Entidaddd</t>
+  </si>
+  <si>
+    <t>Azul</t>
+  </si>
+  <si>
+    <t>entity3@hotmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,12 +140,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,14 +166,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -436,126 +485,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>123456</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="5">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="1"/>
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="5"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="1"/>
-      <c r="J3" s="1"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>123456</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="1"/>
-      <c r="J4" s="1"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>123456</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D5" s="5"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="1"/>
-      <c r="J5" s="1"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>123456</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D6" s="5"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="1"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>123456</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
+    <hyperlink ref="H4" r:id="rId3"/>
+    <hyperlink ref="H5" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Arreglado el lector de CSV
Antes estaba comentado, porque no funcionaba bien.
</commit_message>
<xml_diff>
--- a/src/test/resources/test1.xlsx
+++ b/src/test/resources/test1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19845" windowHeight="5025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21660" windowHeight="4695"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Contrasena</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>entity3@hotmail.com</t>
+  </si>
+  <si>
+    <t>Entityi</t>
+  </si>
+  <si>
+    <t>EntidadTipoErroneo</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,10 +634,10 @@
         <v>123456</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D6">
         <v>2</v>

</xml_diff>